<commit_message>
Updated merged with some fix of missing values and additional locals
</commit_message>
<xml_diff>
--- a/MergedDataset.xlsx
+++ b/MergedDataset.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -393,50 +393,80 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>us_confirmed</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>us_recovered</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>us_death</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>newyork_confirmed</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>newyork_recovered</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>newyork_death</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>denmark_confirmed</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>denmark_recovered</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>denmark_death</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>tompkins_pending_tests</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>tompkins_confirmed</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>tompkins_negative</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Total_tested</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>tompkins_quarantined</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Released_quarantine</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>tompkins_death</t>
         </is>
@@ -459,13 +489,13 @@
         <v>2996</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -477,7 +507,7 @@
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -486,6 +516,24 @@
         <v>0</v>
       </c>
       <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -506,13 +554,13 @@
         <v>3085</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -524,7 +572,7 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -533,6 +581,24 @@
         <v>0</v>
       </c>
       <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -553,13 +619,13 @@
         <v>3160</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
@@ -571,7 +637,7 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -580,6 +646,24 @@
         <v>0</v>
       </c>
       <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -600,13 +684,13 @@
         <v>3254</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -618,7 +702,7 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -627,6 +711,24 @@
         <v>0</v>
       </c>
       <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -647,13 +749,13 @@
         <v>3348</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>221</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -665,7 +767,7 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
@@ -674,6 +776,24 @@
         <v>0</v>
       </c>
       <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -694,13 +814,13 @@
         <v>3460</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>278</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -712,15 +832,33 @@
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" t="n">
         <v>0</v>
       </c>
       <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -741,13 +879,13 @@
         <v>3558</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>417</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -759,15 +897,33 @@
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" t="n">
         <v>0</v>
       </c>
       <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -788,13 +944,13 @@
         <v>3803</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>537</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -806,15 +962,33 @@
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" t="n">
         <v>0</v>
       </c>
       <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -835,13 +1009,13 @@
         <v>3996</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>605</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -853,15 +1027,33 @@
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
       </c>
       <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -882,17 +1074,17 @@
         <v>4262</v>
       </c>
       <c r="F11" t="n">
+        <v>959</v>
+      </c>
+      <c r="G11" t="n">
+        <v>8</v>
+      </c>
+      <c r="H11" t="n">
+        <v>28</v>
+      </c>
+      <c r="I11" t="n">
         <v>173</v>
       </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
       <c r="J11" t="n">
         <v>0</v>
       </c>
@@ -900,15 +1092,33 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>262</v>
       </c>
       <c r="M11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" t="n">
         <v>0</v>
       </c>
       <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -929,17 +1139,17 @@
         <v>4615</v>
       </c>
       <c r="F12" t="n">
+        <v>1281</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8</v>
+      </c>
+      <c r="H12" t="n">
+        <v>36</v>
+      </c>
+      <c r="I12" t="n">
         <v>220</v>
       </c>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
       <c r="J12" t="n">
         <v>0</v>
       </c>
@@ -947,15 +1157,33 @@
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>444</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
       </c>
       <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -976,17 +1204,17 @@
         <v>4720</v>
       </c>
       <c r="F13" t="n">
+        <v>1663</v>
+      </c>
+      <c r="G13" t="n">
+        <v>12</v>
+      </c>
+      <c r="H13" t="n">
+        <v>40</v>
+      </c>
+      <c r="I13" t="n">
         <v>328</v>
       </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
       <c r="J13" t="n">
         <v>0</v>
       </c>
@@ -994,15 +1222,33 @@
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>617</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" t="n">
         <v>0</v>
       </c>
       <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0</v>
+      </c>
+      <c r="U13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1023,17 +1269,17 @@
         <v>5404</v>
       </c>
       <c r="F14" t="n">
+        <v>2179</v>
+      </c>
+      <c r="G14" t="n">
+        <v>12</v>
+      </c>
+      <c r="H14" t="n">
+        <v>47</v>
+      </c>
+      <c r="I14" t="n">
         <v>421</v>
       </c>
-      <c r="G14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
       <c r="J14" t="n">
         <v>0</v>
       </c>
@@ -1041,15 +1287,33 @@
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>804</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
       </c>
       <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1070,33 +1334,51 @@
         <v>5819</v>
       </c>
       <c r="F15" t="n">
+        <v>2726</v>
+      </c>
+      <c r="G15" t="n">
+        <v>12</v>
+      </c>
+      <c r="H15" t="n">
+        <v>54</v>
+      </c>
+      <c r="I15" t="n">
         <v>525</v>
       </c>
-      <c r="G15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" t="n">
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
         <v>2</v>
       </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
       <c r="L15" t="n">
-        <v>0</v>
+        <v>836</v>
       </c>
       <c r="M15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>0</v>
+      </c>
+      <c r="U15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1117,33 +1399,51 @@
         <v>6440</v>
       </c>
       <c r="F16" t="n">
+        <v>3499</v>
+      </c>
+      <c r="G16" t="n">
+        <v>12</v>
+      </c>
+      <c r="H16" t="n">
+        <v>63</v>
+      </c>
+      <c r="I16" t="n">
         <v>732</v>
       </c>
-      <c r="G16" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" t="n">
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
         <v>3</v>
       </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
       <c r="L16" t="n">
-        <v>0</v>
+        <v>875</v>
       </c>
       <c r="M16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O16" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1164,33 +1464,51 @@
         <v>7126</v>
       </c>
       <c r="F17" t="n">
+        <v>4632</v>
+      </c>
+      <c r="G17" t="n">
+        <v>17</v>
+      </c>
+      <c r="H17" t="n">
+        <v>85</v>
+      </c>
+      <c r="I17" t="n">
         <v>967</v>
       </c>
-      <c r="G17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" t="n">
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
         <v>10</v>
       </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0</v>
-      </c>
       <c r="L17" t="n">
-        <v>0</v>
+        <v>932</v>
       </c>
       <c r="M17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O17" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0</v>
+      </c>
+      <c r="U17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1211,33 +1529,51 @@
         <v>7905</v>
       </c>
       <c r="F18" t="n">
+        <v>6421</v>
+      </c>
+      <c r="G18" t="n">
+        <v>17</v>
+      </c>
+      <c r="H18" t="n">
+        <v>108</v>
+      </c>
+      <c r="I18" t="n">
         <v>1706</v>
       </c>
-      <c r="G18" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" t="n">
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" t="n">
         <v>13</v>
       </c>
-      <c r="I18" t="n">
+      <c r="L18" t="n">
+        <v>1024</v>
+      </c>
+      <c r="M18" t="n">
+        <v>1</v>
+      </c>
+      <c r="N18" t="n">
+        <v>4</v>
+      </c>
+      <c r="O18" t="n">
         <v>69</v>
       </c>
-      <c r="J18" t="n">
+      <c r="P18" t="n">
         <v>3</v>
       </c>
-      <c r="K18" t="n">
+      <c r="Q18" t="n">
         <v>35</v>
       </c>
-      <c r="L18" t="n">
+      <c r="R18" t="n">
         <v>107</v>
       </c>
-      <c r="M18" t="n">
+      <c r="S18" t="n">
         <v>82</v>
       </c>
-      <c r="N18" t="n">
+      <c r="T18" t="n">
         <v>35</v>
       </c>
-      <c r="O18" t="n">
+      <c r="U18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1258,33 +1594,51 @@
         <v>8733</v>
       </c>
       <c r="F19" t="n">
+        <v>7786</v>
+      </c>
+      <c r="G19" t="n">
+        <v>106</v>
+      </c>
+      <c r="H19" t="n">
+        <v>118</v>
+      </c>
+      <c r="I19" t="n">
         <v>2495</v>
       </c>
-      <c r="G19" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" t="n">
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
         <v>16</v>
       </c>
-      <c r="I19" t="n">
+      <c r="L19" t="n">
+        <v>1115</v>
+      </c>
+      <c r="M19" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" t="n">
+        <v>4</v>
+      </c>
+      <c r="O19" t="n">
         <v>93</v>
       </c>
-      <c r="J19" t="n">
+      <c r="P19" t="n">
         <v>6</v>
       </c>
-      <c r="K19" t="n">
+      <c r="Q19" t="n">
         <v>46</v>
       </c>
-      <c r="L19" t="n">
+      <c r="R19" t="n">
         <v>146</v>
       </c>
-      <c r="M19" t="n">
+      <c r="S19" t="n">
         <v>86</v>
       </c>
-      <c r="N19" t="n">
+      <c r="T19" t="n">
         <v>35</v>
       </c>
-      <c r="O19" t="n">
+      <c r="U19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1305,33 +1659,51 @@
         <v>9867</v>
       </c>
       <c r="F20" t="n">
+        <v>13680</v>
+      </c>
+      <c r="G20" t="n">
+        <v>108</v>
+      </c>
+      <c r="H20" t="n">
+        <v>200</v>
+      </c>
+      <c r="I20" t="n">
         <v>5365</v>
       </c>
-      <c r="G20" t="n">
-        <v>0</v>
-      </c>
-      <c r="H20" t="n">
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" t="n">
         <v>34</v>
       </c>
-      <c r="I20" t="n">
+      <c r="L20" t="n">
+        <v>1225</v>
+      </c>
+      <c r="M20" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" t="n">
+        <v>6</v>
+      </c>
+      <c r="O20" t="n">
         <v>224</v>
       </c>
-      <c r="J20" t="n">
+      <c r="P20" t="n">
         <v>6</v>
       </c>
-      <c r="K20" t="n">
+      <c r="Q20" t="n">
         <v>49</v>
       </c>
-      <c r="L20" t="n">
+      <c r="R20" t="n">
         <v>279</v>
       </c>
-      <c r="M20" t="n">
+      <c r="S20" t="n">
         <v>293</v>
       </c>
-      <c r="N20" t="n">
+      <c r="T20" t="n">
         <v>57</v>
       </c>
-      <c r="O20" t="n">
+      <c r="U20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1352,33 +1724,51 @@
         <v>11299</v>
       </c>
       <c r="F21" t="n">
+        <v>19101</v>
+      </c>
+      <c r="G21" t="n">
+        <v>147</v>
+      </c>
+      <c r="H21" t="n">
+        <v>244</v>
+      </c>
+      <c r="I21" t="n">
         <v>8310</v>
       </c>
-      <c r="G21" t="n">
-        <v>0</v>
-      </c>
-      <c r="H21" t="n">
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" t="n">
         <v>42</v>
       </c>
-      <c r="I21" t="n">
+      <c r="L21" t="n">
+        <v>1337</v>
+      </c>
+      <c r="M21" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" t="n">
+        <v>9</v>
+      </c>
+      <c r="O21" t="n">
         <v>280</v>
       </c>
-      <c r="J21" t="n">
+      <c r="P21" t="n">
         <v>11</v>
       </c>
-      <c r="K21" t="n">
+      <c r="Q21" t="n">
         <v>88</v>
       </c>
-      <c r="L21" t="n">
+      <c r="R21" t="n">
         <v>379</v>
       </c>
-      <c r="M21" t="n">
+      <c r="S21" t="n">
         <v>515</v>
       </c>
-      <c r="N21" t="n">
+      <c r="T21" t="n">
         <v>153</v>
       </c>
-      <c r="O21" t="n">
+      <c r="U21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1399,33 +1789,51 @@
         <v>12973</v>
       </c>
       <c r="F22" t="n">
+        <v>25493</v>
+      </c>
+      <c r="G22" t="n">
+        <v>171</v>
+      </c>
+      <c r="H22" t="n">
+        <v>307</v>
+      </c>
+      <c r="I22" t="n">
         <v>11710</v>
       </c>
-      <c r="G22" t="n">
-        <v>0</v>
-      </c>
-      <c r="H22" t="n">
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="n">
         <v>60</v>
       </c>
-      <c r="I22" t="n">
+      <c r="L22" t="n">
+        <v>1420</v>
+      </c>
+      <c r="M22" t="n">
+        <v>1</v>
+      </c>
+      <c r="N22" t="n">
+        <v>13</v>
+      </c>
+      <c r="O22" t="n">
         <v>302</v>
       </c>
-      <c r="J22" t="n">
+      <c r="P22" t="n">
         <v>12</v>
       </c>
-      <c r="K22" t="n">
+      <c r="Q22" t="n">
         <v>135</v>
       </c>
-      <c r="L22" t="n">
+      <c r="R22" t="n">
         <v>449</v>
       </c>
-      <c r="M22" t="n">
+      <c r="S22" t="n">
         <v>418</v>
       </c>
-      <c r="N22" t="n">
+      <c r="T22" t="n">
         <v>206</v>
       </c>
-      <c r="O22" t="n">
+      <c r="U22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1446,33 +1854,51 @@
         <v>14623</v>
       </c>
       <c r="F23" t="n">
+        <v>33746</v>
+      </c>
+      <c r="G23" t="n">
+        <v>171</v>
+      </c>
+      <c r="H23" t="n">
+        <v>427</v>
+      </c>
+      <c r="I23" t="n">
         <v>15800</v>
       </c>
-      <c r="G23" t="n">
-        <v>0</v>
-      </c>
-      <c r="H23" t="n">
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
         <v>117</v>
       </c>
-      <c r="I23" t="n">
+      <c r="L23" t="n">
+        <v>1514</v>
+      </c>
+      <c r="M23" t="n">
+        <v>4</v>
+      </c>
+      <c r="N23" t="n">
+        <v>13</v>
+      </c>
+      <c r="O23" t="n">
         <v>276</v>
       </c>
-      <c r="J23" t="n">
+      <c r="P23" t="n">
         <v>15</v>
       </c>
-      <c r="K23" t="n">
+      <c r="Q23" t="n">
         <v>160</v>
       </c>
-      <c r="L23" t="n">
+      <c r="R23" t="n">
         <v>451</v>
       </c>
-      <c r="M23" t="n">
+      <c r="S23" t="n">
         <v>397</v>
       </c>
-      <c r="N23" t="n">
+      <c r="T23" t="n">
         <v>235</v>
       </c>
-      <c r="O23" t="n">
+      <c r="U23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1493,33 +1919,51 @@
         <v>16497</v>
       </c>
       <c r="F24" t="n">
+        <v>43667</v>
+      </c>
+      <c r="G24" t="n">
+        <v>171</v>
+      </c>
+      <c r="H24" t="n">
+        <v>552</v>
+      </c>
+      <c r="I24" t="n">
         <v>20884</v>
       </c>
-      <c r="G24" t="n">
-        <v>0</v>
-      </c>
-      <c r="H24" t="n">
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="n">
         <v>158</v>
       </c>
-      <c r="I24" t="n">
+      <c r="L24" t="n">
+        <v>1572</v>
+      </c>
+      <c r="M24" t="n">
+        <v>24</v>
+      </c>
+      <c r="N24" t="n">
+        <v>24</v>
+      </c>
+      <c r="O24" t="n">
         <v>251</v>
       </c>
-      <c r="J24" t="n">
+      <c r="P24" t="n">
         <v>16</v>
       </c>
-      <c r="K24" t="n">
+      <c r="Q24" t="n">
         <v>325</v>
       </c>
-      <c r="L24" t="n">
+      <c r="R24" t="n">
         <v>592</v>
       </c>
-      <c r="M24" t="n">
+      <c r="S24" t="n">
         <v>244</v>
       </c>
-      <c r="N24" t="n">
+      <c r="T24" t="n">
         <v>344</v>
       </c>
-      <c r="O24" t="n">
+      <c r="U24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1540,33 +1984,51 @@
         <v>18615</v>
       </c>
       <c r="F25" t="n">
+        <v>53740</v>
+      </c>
+      <c r="G25" t="n">
+        <v>348</v>
+      </c>
+      <c r="H25" t="n">
+        <v>706</v>
+      </c>
+      <c r="I25" t="n">
         <v>25681</v>
       </c>
-      <c r="G25" t="n">
-        <v>0</v>
-      </c>
-      <c r="H25" t="n">
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="n">
         <v>210</v>
       </c>
-      <c r="I25" t="n">
+      <c r="L25" t="n">
+        <v>1718</v>
+      </c>
+      <c r="M25" t="n">
+        <v>36</v>
+      </c>
+      <c r="N25" t="n">
+        <v>32</v>
+      </c>
+      <c r="O25" t="n">
         <v>218</v>
       </c>
-      <c r="J25" t="n">
+      <c r="P25" t="n">
         <v>18</v>
       </c>
-      <c r="K25" t="n">
+      <c r="Q25" t="n">
         <v>430</v>
       </c>
-      <c r="L25" t="n">
+      <c r="R25" t="n">
         <v>666</v>
       </c>
-      <c r="M25" t="n">
+      <c r="S25" t="n">
         <v>326</v>
       </c>
-      <c r="N25" t="n">
+      <c r="T25" t="n">
         <v>441</v>
       </c>
-      <c r="O25" t="n">
+      <c r="U25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1587,33 +2049,116 @@
         <v>21181</v>
       </c>
       <c r="F26" t="n">
+        <v>65778</v>
+      </c>
+      <c r="G26" t="n">
+        <v>361</v>
+      </c>
+      <c r="H26" t="n">
+        <v>942</v>
+      </c>
+      <c r="I26" t="n">
         <v>30841</v>
       </c>
-      <c r="G26" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" t="n">
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="n">
         <v>285</v>
       </c>
-      <c r="I26" t="n">
+      <c r="L26" t="n">
+        <v>1862</v>
+      </c>
+      <c r="M26" t="n">
+        <v>41</v>
+      </c>
+      <c r="N26" t="n">
+        <v>34</v>
+      </c>
+      <c r="O26" t="n">
         <v>236</v>
       </c>
-      <c r="J26" t="n">
+      <c r="P26" t="n">
         <v>23</v>
       </c>
-      <c r="K26" t="n">
+      <c r="Q26" t="n">
         <v>472</v>
       </c>
-      <c r="L26" t="n">
+      <c r="R26" t="n">
         <v>731</v>
       </c>
-      <c r="M26" t="n">
+      <c r="S26" t="n">
         <v>351</v>
       </c>
-      <c r="N26" t="n">
+      <c r="T26" t="n">
         <v>484</v>
       </c>
-      <c r="O26" t="n">
+      <c r="U26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>43916</v>
+      </c>
+      <c r="C27" t="n">
+        <v>529591</v>
+      </c>
+      <c r="D27" t="n">
+        <v>122150</v>
+      </c>
+      <c r="E27" t="n">
+        <v>23970</v>
+      </c>
+      <c r="F27" t="n">
+        <v>83836</v>
+      </c>
+      <c r="G27" t="n">
+        <v>681</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1209</v>
+      </c>
+      <c r="I27" t="n">
+        <v>37877</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
+        <v>385</v>
+      </c>
+      <c r="L27" t="n">
+        <v>2023</v>
+      </c>
+      <c r="M27" t="n">
+        <v>50</v>
+      </c>
+      <c r="N27" t="n">
+        <v>41</v>
+      </c>
+      <c r="O27" t="n">
+        <v>462</v>
+      </c>
+      <c r="P27" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>515</v>
+      </c>
+      <c r="R27" t="n">
+        <v>1009</v>
+      </c>
+      <c r="S27" t="n">
+        <v>354</v>
+      </c>
+      <c r="T27" t="n">
+        <v>526</v>
+      </c>
+      <c r="U27" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tompkins health update - other data for today pending
Tompkins Update -
Quarantined numbers no longer reported
Other data pending.
</commit_message>
<xml_diff>
--- a/MergedDataset.xlsx
+++ b/MergedDataset.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U27"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2162,6 +2162,71 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" t="n">
+        <v>628</v>
+      </c>
+      <c r="P28" t="n">
+        <v>48</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>515</v>
+      </c>
+      <c r="R28" t="n">
+        <v>1191</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0</v>
+      </c>
+      <c r="U28" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
TCHD data updated - other merged data pending.
As of 03/29/20 at 5:00 pm. Source: TCHD
</commit_message>
<xml_diff>
--- a/MergedDataset.xlsx
+++ b/MergedDataset.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V29"/>
+  <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2366,7 +2366,7 @@
         <v>624</v>
       </c>
       <c r="R29" t="n">
-        <v>0</v>
+        <v>1191</v>
       </c>
       <c r="S29" t="n">
         <v>0</v>
@@ -2378,6 +2378,74 @@
         <v>0</v>
       </c>
       <c r="V29" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" t="n">
+        <v>70</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>996</v>
+      </c>
+      <c r="R30" t="n">
+        <v>1197</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0</v>
+      </c>
+      <c r="V30" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
merged data updated for today
</commit_message>
<xml_diff>
--- a/MergedDataset.xlsx
+++ b/MergedDataset.xlsx
@@ -2385,44 +2385,44 @@
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30" t="n">
-        <v>0</v>
+      <c r="B30" s="2" t="n">
+        <v>43919</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>720117</v>
       </c>
       <c r="D30" t="n">
-        <v>0</v>
+        <v>149082</v>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>33925</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>140886</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>2665</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>2467</v>
       </c>
       <c r="I30" t="n">
-        <v>0</v>
+        <v>59648</v>
       </c>
       <c r="J30" t="n">
         <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>965</v>
       </c>
       <c r="L30" t="n">
-        <v>0</v>
+        <v>2564</v>
       </c>
       <c r="M30" t="n">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="N30" t="n">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="O30" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Update for March 30, 2020
</commit_message>
<xml_diff>
--- a/MergedDataset.xlsx
+++ b/MergedDataset.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V30"/>
+  <dimension ref="A1:W31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,11 @@
           <t>tompkins_currently_hospitalized</t>
         </is>
       </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>tompkins_discharged_from_hospital</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -542,6 +547,9 @@
         <v>0</v>
       </c>
       <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -612,6 +620,9 @@
       <c r="V3" t="n">
         <v>0</v>
       </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -680,6 +691,9 @@
       <c r="V4" t="n">
         <v>0</v>
       </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -748,6 +762,9 @@
       <c r="V5" t="n">
         <v>0</v>
       </c>
+      <c r="W5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -816,6 +833,9 @@
       <c r="V6" t="n">
         <v>0</v>
       </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -884,6 +904,9 @@
       <c r="V7" t="n">
         <v>0</v>
       </c>
+      <c r="W7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -952,6 +975,9 @@
       <c r="V8" t="n">
         <v>0</v>
       </c>
+      <c r="W8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1020,6 +1046,9 @@
       <c r="V9" t="n">
         <v>0</v>
       </c>
+      <c r="W9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1088,6 +1117,9 @@
       <c r="V10" t="n">
         <v>0</v>
       </c>
+      <c r="W10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1156,6 +1188,9 @@
       <c r="V11" t="n">
         <v>0</v>
       </c>
+      <c r="W11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1224,6 +1259,9 @@
       <c r="V12" t="n">
         <v>0</v>
       </c>
+      <c r="W12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1292,6 +1330,9 @@
       <c r="V13" t="n">
         <v>0</v>
       </c>
+      <c r="W13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1360,6 +1401,9 @@
       <c r="V14" t="n">
         <v>0</v>
       </c>
+      <c r="W14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1428,6 +1472,9 @@
       <c r="V15" t="n">
         <v>0</v>
       </c>
+      <c r="W15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1496,6 +1543,9 @@
       <c r="V16" t="n">
         <v>0</v>
       </c>
+      <c r="W16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1564,6 +1614,9 @@
       <c r="V17" t="n">
         <v>0</v>
       </c>
+      <c r="W17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1632,6 +1685,9 @@
       <c r="V18" t="n">
         <v>0</v>
       </c>
+      <c r="W18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1700,6 +1756,9 @@
       <c r="V19" t="n">
         <v>0</v>
       </c>
+      <c r="W19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1768,6 +1827,9 @@
       <c r="V20" t="n">
         <v>0</v>
       </c>
+      <c r="W20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1836,6 +1898,9 @@
       <c r="V21" t="n">
         <v>0</v>
       </c>
+      <c r="W21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1904,6 +1969,9 @@
       <c r="V22" t="n">
         <v>0</v>
       </c>
+      <c r="W22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1972,6 +2040,9 @@
       <c r="V23" t="n">
         <v>0</v>
       </c>
+      <c r="W23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -2040,6 +2111,9 @@
       <c r="V24" t="n">
         <v>0</v>
       </c>
+      <c r="W24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -2108,6 +2182,9 @@
       <c r="V25" t="n">
         <v>0</v>
       </c>
+      <c r="W25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -2176,6 +2253,9 @@
       <c r="V26" t="n">
         <v>0</v>
       </c>
+      <c r="W26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -2244,6 +2324,9 @@
       <c r="V27" t="n">
         <v>0</v>
       </c>
+      <c r="W27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2312,6 +2395,9 @@
       <c r="V28" t="n">
         <v>0</v>
       </c>
+      <c r="W28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2380,6 +2466,9 @@
       <c r="V29" t="n">
         <v>2</v>
       </c>
+      <c r="W29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2447,6 +2536,80 @@
       </c>
       <c r="V30" t="n">
         <v>2</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>43920</v>
+      </c>
+      <c r="C31" t="n">
+        <v>782365</v>
+      </c>
+      <c r="D31" t="n">
+        <v>164566</v>
+      </c>
+      <c r="E31" t="n">
+        <v>37582</v>
+      </c>
+      <c r="F31" t="n">
+        <v>161807</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5644</v>
+      </c>
+      <c r="H31" t="n">
+        <v>2978</v>
+      </c>
+      <c r="I31" t="n">
+        <v>66663</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>1218</v>
+      </c>
+      <c r="L31" t="n">
+        <v>2755</v>
+      </c>
+      <c r="M31" t="n">
+        <v>73</v>
+      </c>
+      <c r="N31" t="n">
+        <v>77</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" t="n">
+        <v>73</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>1096</v>
+      </c>
+      <c r="R31" t="n">
+        <v>1427</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0</v>
+      </c>
+      <c r="V31" t="n">
+        <v>1</v>
+      </c>
+      <c r="W31" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TCHD update included. Merged data pending update.
</commit_message>
<xml_diff>
--- a/MergedDataset.xlsx
+++ b/MergedDataset.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y32"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2846,7 +2846,7 @@
         <v>90</v>
       </c>
       <c r="O32" t="n">
-        <v>0</v>
+        <v>242</v>
       </c>
       <c r="P32" t="n">
         <v>76</v>
@@ -2877,6 +2877,83 @@
       </c>
       <c r="Y32" t="n">
         <v>28</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>242</v>
+      </c>
+      <c r="P33" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>1158</v>
+      </c>
+      <c r="R33" t="n">
+        <v>1480</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0</v>
+      </c>
+      <c r="V33" t="n">
+        <v>1</v>
+      </c>
+      <c r="W33" t="n">
+        <v>1</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update with yesterdays data
</commit_message>
<xml_diff>
--- a/MergedDataset.xlsx
+++ b/MergedDataset.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3033,6 +3033,83 @@
         <v>46</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="n">
+        <v>43924</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1095917</v>
+      </c>
+      <c r="D35" t="n">
+        <v>225796</v>
+      </c>
+      <c r="E35" t="n">
+        <v>58787</v>
+      </c>
+      <c r="F35" t="n">
+        <v>275586</v>
+      </c>
+      <c r="G35" t="n">
+        <v>9707</v>
+      </c>
+      <c r="H35" t="n">
+        <v>7087</v>
+      </c>
+      <c r="I35" t="n">
+        <v>102987</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
+      <c r="K35" t="n">
+        <v>2935</v>
+      </c>
+      <c r="L35" t="n">
+        <v>3946</v>
+      </c>
+      <c r="M35" t="n">
+        <v>1287</v>
+      </c>
+      <c r="N35" t="n">
+        <v>139</v>
+      </c>
+      <c r="O35" t="n">
+        <v>164</v>
+      </c>
+      <c r="P35" t="n">
+        <v>93</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>1363</v>
+      </c>
+      <c r="R35" t="n">
+        <v>1620</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" t="n">
+        <v>2</v>
+      </c>
+      <c r="W35" t="n">
+        <v>1</v>
+      </c>
+      <c r="X35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
tompkins data updated for 2020_4_4, other data pending.
</commit_message>
<xml_diff>
--- a/MergedDataset.xlsx
+++ b/MergedDataset.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y35"/>
+  <dimension ref="A1:Y36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3110,6 +3110,83 @@
         <v>51</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" t="n">
+        <v>105</v>
+      </c>
+      <c r="P36" t="n">
+        <v>95</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>1426</v>
+      </c>
+      <c r="R36" t="n">
+        <v>1626</v>
+      </c>
+      <c r="S36" t="n">
+        <v>0</v>
+      </c>
+      <c r="T36" t="n">
+        <v>0</v>
+      </c>
+      <c r="U36" t="n">
+        <v>0</v>
+      </c>
+      <c r="V36" t="n">
+        <v>2</v>
+      </c>
+      <c r="W36" t="n">
+        <v>1</v>
+      </c>
+      <c r="X36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
tompkins updated 2020_04_06, rest of merged data pending
</commit_message>
<xml_diff>
--- a/MergedDataset.xlsx
+++ b/MergedDataset.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y37"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3264,6 +3264,83 @@
         <v>57</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0</v>
+      </c>
+      <c r="L38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0</v>
+      </c>
+      <c r="O38" t="n">
+        <v>430</v>
+      </c>
+      <c r="P38" t="n">
+        <v>102</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>1456</v>
+      </c>
+      <c r="R38" t="n">
+        <v>1988</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0</v>
+      </c>
+      <c r="T38" t="n">
+        <v>0</v>
+      </c>
+      <c r="U38" t="n">
+        <v>0</v>
+      </c>
+      <c r="V38" t="n">
+        <v>3</v>
+      </c>
+      <c r="W38" t="n">
+        <v>2</v>
+      </c>
+      <c r="X38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
merged data update 2020_04_06
</commit_message>
<xml_diff>
--- a/MergedDataset.xlsx
+++ b/MergedDataset.xlsx
@@ -3268,44 +3268,44 @@
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38" t="n">
-        <v>0</v>
+      <c r="B38" s="2" t="n">
+        <v>43927</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>1345048</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>276515</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>74565</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>366614</v>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>19581</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>10783</v>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>131815</v>
       </c>
       <c r="J38" t="n">
         <v>0</v>
       </c>
       <c r="K38" t="n">
-        <v>0</v>
+        <v>4698</v>
       </c>
       <c r="L38" t="n">
-        <v>0</v>
+        <v>4875</v>
       </c>
       <c r="M38" t="n">
-        <v>0</v>
+        <v>1489</v>
       </c>
       <c r="N38" t="n">
-        <v>0</v>
+        <v>187</v>
       </c>
       <c r="O38" t="n">
         <v>430</v>

</xml_diff>

<commit_message>
Tompkins update - rest of data pending
Note: Looks like one test result is back today and that is positive. Many more pending. Results from these could come in 2-4 days. Expect many more positives this week. We'll see.
</commit_message>
<xml_diff>
--- a/MergedDataset.xlsx
+++ b/MergedDataset.xlsx
@@ -362,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y38"/>
+  <dimension ref="A1:Y39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3272,7 +3272,7 @@
         <v>43927</v>
       </c>
       <c r="C38" t="n">
-        <v>1345048</v>
+        <v>1345101</v>
       </c>
       <c r="D38" t="n">
         <v>276515</v>
@@ -3281,7 +3281,7 @@
         <v>74565</v>
       </c>
       <c r="F38" t="n">
-        <v>366614</v>
+        <v>366667</v>
       </c>
       <c r="G38" t="n">
         <v>19581</v>
@@ -3339,6 +3339,83 @@
       </c>
       <c r="Y38" t="n">
         <v>66</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
+        <v>0</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
+        <v>0</v>
+      </c>
+      <c r="O39" t="n">
+        <v>574</v>
+      </c>
+      <c r="P39" t="n">
+        <v>103</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>1456</v>
+      </c>
+      <c r="R39" t="n">
+        <v>2133</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0</v>
+      </c>
+      <c r="T39" t="n">
+        <v>0</v>
+      </c>
+      <c r="U39" t="n">
+        <v>0</v>
+      </c>
+      <c r="V39" t="n">
+        <v>3</v>
+      </c>
+      <c r="W39" t="n">
+        <v>2</v>
+      </c>
+      <c r="X39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>